<commit_message>
update các dữ liệu master
</commit_message>
<xml_diff>
--- a/public/excel/CustomerPartner.xlsx
+++ b/public/excel/CustomerPartner.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TLG\DeliveryTracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft.public\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>LV2</t>
   </si>
@@ -35,13 +35,16 @@
     <t>LV4</t>
   </si>
   <si>
-    <t>Tên KH</t>
-  </si>
-  <si>
     <t>Mã KH</t>
   </si>
   <si>
     <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Key KH</t>
+  </si>
+  <si>
+    <t>Nhóm khách hàng</t>
   </si>
 </sst>
 </file>
@@ -65,7 +68,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -76,12 +79,6 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -134,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -145,12 +142,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,332 +422,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F38"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="2" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="9"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="9"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="9"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="9"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="9"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="9"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update file excel cho khách hàng đối tác
</commit_message>
<xml_diff>
--- a/public/excel/CustomerPartner.xlsx
+++ b/public/excel/CustomerPartner.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft.public\Downloads\"/>
@@ -12,19 +12,26 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Nhóm khách hàng</t>
+  </si>
+  <si>
+    <t>Khác hàng key</t>
+  </si>
+  <si>
+    <t>Mã khách hàng</t>
+  </si>
+  <si>
+    <t>Ghi chú</t>
+  </si>
   <si>
     <t>LV2</t>
   </si>
@@ -35,16 +42,13 @@
     <t>LV4</t>
   </si>
   <si>
-    <t>Mã KH</t>
-  </si>
-  <si>
-    <t>Ghi chú</t>
-  </si>
-  <si>
-    <t>Key KH</t>
-  </si>
-  <si>
-    <t>Nhóm khách hàng</t>
+    <t>Fujimart</t>
+  </si>
+  <si>
+    <t>11041 Siªu thÞ FujiMart Huúnh Thóc Kh¸ng</t>
+  </si>
+  <si>
+    <t>FujiMart Huỳnh Thúc Kháng (Hà Nội)</t>
   </si>
 </sst>
 </file>
@@ -54,18 +58,14 @@
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -77,12 +77,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor theme="4"/>
+        <fgColor rgb="FFB0C4DE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -92,38 +92,16 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FF000000"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -131,23 +109,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -170,44 +142,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -240,9 +212,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -281,179 +253,231 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="60" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="5" max="6" width="4" customWidth="1"/>
+    <col min="7" max="7" width="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>2</v>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>104218</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>302</v>
+      </c>
+      <c r="F2">
+        <v>377</v>
+      </c>
+      <c r="G2">
+        <v>1440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>